<commit_message>
modified:   BOM/BOM.csv 	modified:   BOM/BOM.xlsx 	modified:   README.md
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wiktr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C95073-D9D1-40B7-8A67-F38959BB587A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C302F4E-BEAE-4163-9F8C-24BE6A638585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A30D2B41-88E1-43CC-A132-183753402AA5}"/>
   </bookViews>
@@ -177,7 +177,7 @@
     <t>TOTAL ESTIMATED PROJECT COST:</t>
   </si>
   <si>
-    <t>~$390 - $455</t>
+    <t>~$390 - $400</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>